<commit_message>
add the win10 11.2
</commit_message>
<xml_diff>
--- a/python/two_band/回测.xlsx
+++ b/python/two_band/回测.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="121">
   <si>
     <t>rb1801</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -421,6 +421,82 @@
   </si>
   <si>
     <t>limit——volume——（5秒，2）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>次数用完了，没有抓到上涨趋势</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上涨趋势用完了，没有抓到上涨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下跌趋势用完了，没有抓到下跌趋势</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下跌趋势用完了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开单天数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>盈利天数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>盈利tick数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>次数用完没有抓到趋势</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>limit_volume</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>盈利tick数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>次数用完，没有到趋势</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>limit_triggersize最大损失10个tick</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>次数用完了，没有抓到趋势</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -464,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -472,6 +548,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -776,17 +853,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BE154"/>
+  <dimension ref="A1:BE219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B142" workbookViewId="0">
-      <selection activeCell="N147" sqref="N147"/>
+    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="E216" sqref="E216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="4" max="12" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="31" width="17.25" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.875" customWidth="1"/>
+    <col min="6" max="12" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
+    <col min="14" max="31" width="17.25" customWidth="1"/>
     <col min="32" max="32" width="17.5" customWidth="1"/>
     <col min="33" max="35" width="17.25" customWidth="1"/>
     <col min="36" max="57" width="9.5" bestFit="1" customWidth="1"/>
@@ -6913,7 +6993,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="145" spans="1:56" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:57" x14ac:dyDescent="0.15">
       <c r="D145">
         <v>7</v>
       </c>
@@ -6981,7 +7061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:56" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:57" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.15">
       <c r="J146" s="1" t="s">
         <v>99</v>
       </c>
@@ -7031,7 +7111,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="147" spans="1:56" ht="27" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:57" ht="27" x14ac:dyDescent="0.15">
       <c r="B147" s="1" t="s">
         <v>97</v>
       </c>
@@ -7096,7 +7176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:56" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:57" x14ac:dyDescent="0.15">
       <c r="B148" s="1"/>
       <c r="D148">
         <v>6</v>
@@ -7114,7 +7194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:56" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:57" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B149" s="1" t="s">
         <v>100</v>
       </c>
@@ -7179,7 +7259,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="150" spans="1:56" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:57" x14ac:dyDescent="0.15">
       <c r="B150" s="1"/>
       <c r="D150">
         <v>4</v>
@@ -7242,10 +7322,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:56" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:57" x14ac:dyDescent="0.15">
       <c r="B151" s="1"/>
     </row>
-    <row r="152" spans="1:56" ht="27" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:57" ht="27" x14ac:dyDescent="0.15">
       <c r="A152" s="1" t="s">
         <v>90</v>
       </c>
@@ -7262,7 +7342,7 @@
         <v>-142</v>
       </c>
     </row>
-    <row r="153" spans="1:56" ht="27" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:57" ht="27" x14ac:dyDescent="0.15">
       <c r="D153" s="1" t="s">
         <v>92</v>
       </c>
@@ -7270,7 +7350,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="154" spans="1:56" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:57" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B154" s="1" t="s">
         <v>100</v>
       </c>
@@ -7279,6 +7359,3354 @@
       </c>
       <c r="E154">
         <v>90</v>
+      </c>
+    </row>
+    <row r="157" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="D157">
+        <v>20170807</v>
+      </c>
+      <c r="E157">
+        <v>20170808</v>
+      </c>
+      <c r="F157">
+        <v>20170809</v>
+      </c>
+      <c r="G157">
+        <v>20170810</v>
+      </c>
+      <c r="H157">
+        <v>20170811</v>
+      </c>
+      <c r="I157">
+        <v>20170814</v>
+      </c>
+      <c r="J157">
+        <v>20170815</v>
+      </c>
+      <c r="K157">
+        <v>20170816</v>
+      </c>
+      <c r="L157">
+        <v>20170817</v>
+      </c>
+      <c r="M157">
+        <v>20170818</v>
+      </c>
+      <c r="N157">
+        <v>20170821</v>
+      </c>
+      <c r="O157">
+        <v>20170822</v>
+      </c>
+      <c r="P157">
+        <v>20170823</v>
+      </c>
+      <c r="Q157">
+        <v>20170824</v>
+      </c>
+      <c r="R157">
+        <v>20170825</v>
+      </c>
+      <c r="S157">
+        <v>20170828</v>
+      </c>
+      <c r="T157">
+        <v>20170829</v>
+      </c>
+      <c r="U157">
+        <v>20170830</v>
+      </c>
+      <c r="V157">
+        <v>20170831</v>
+      </c>
+      <c r="W157">
+        <v>20170901</v>
+      </c>
+      <c r="X157">
+        <v>20170904</v>
+      </c>
+      <c r="Y157">
+        <v>20170905</v>
+      </c>
+      <c r="Z157">
+        <v>20170906</v>
+      </c>
+      <c r="AA157">
+        <v>20170907</v>
+      </c>
+      <c r="AB157">
+        <v>20170908</v>
+      </c>
+      <c r="AC157">
+        <v>20170911</v>
+      </c>
+      <c r="AD157">
+        <v>20170912</v>
+      </c>
+      <c r="AE157">
+        <v>20170913</v>
+      </c>
+      <c r="AF157">
+        <v>20170914</v>
+      </c>
+      <c r="AG157">
+        <v>20170915</v>
+      </c>
+      <c r="AH157">
+        <v>20170918</v>
+      </c>
+      <c r="AI157">
+        <v>20170919</v>
+      </c>
+      <c r="AJ157">
+        <v>20170920</v>
+      </c>
+      <c r="AK157">
+        <v>20170921</v>
+      </c>
+      <c r="AL157">
+        <v>20170922</v>
+      </c>
+      <c r="AM157">
+        <v>20170925</v>
+      </c>
+      <c r="AN157">
+        <v>20170926</v>
+      </c>
+      <c r="AO157">
+        <v>20170927</v>
+      </c>
+      <c r="AP157">
+        <v>20170928</v>
+      </c>
+      <c r="AQ157">
+        <v>20170929</v>
+      </c>
+      <c r="AR157">
+        <v>20171009</v>
+      </c>
+      <c r="AS157">
+        <v>20171010</v>
+      </c>
+      <c r="AT157">
+        <v>20171011</v>
+      </c>
+      <c r="AU157">
+        <v>20171012</v>
+      </c>
+      <c r="AV157">
+        <v>20171013</v>
+      </c>
+      <c r="AW157">
+        <v>20171016</v>
+      </c>
+      <c r="AX157">
+        <v>20171017</v>
+      </c>
+      <c r="AY157">
+        <v>20171018</v>
+      </c>
+      <c r="AZ157">
+        <v>20171019</v>
+      </c>
+      <c r="BA157">
+        <v>20171020</v>
+      </c>
+      <c r="BB157">
+        <v>20171023</v>
+      </c>
+      <c r="BC157">
+        <v>20171024</v>
+      </c>
+      <c r="BD157">
+        <v>20171025</v>
+      </c>
+      <c r="BE157">
+        <v>20171026</v>
+      </c>
+    </row>
+    <row r="158" spans="1:57" ht="27" x14ac:dyDescent="0.15">
+      <c r="A158" t="s">
+        <v>102</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H158">
+        <v>50</v>
+      </c>
+      <c r="I158">
+        <v>-38</v>
+      </c>
+      <c r="AA158">
+        <v>33</v>
+      </c>
+      <c r="AB158">
+        <v>106</v>
+      </c>
+      <c r="AD158">
+        <v>44</v>
+      </c>
+      <c r="AE158">
+        <v>212</v>
+      </c>
+      <c r="AO158">
+        <v>41</v>
+      </c>
+      <c r="AQ158">
+        <v>-22</v>
+      </c>
+      <c r="AR158">
+        <v>-18</v>
+      </c>
+      <c r="AS158">
+        <v>-17</v>
+      </c>
+      <c r="AV158">
+        <v>-19</v>
+      </c>
+      <c r="AZ158">
+        <v>-40</v>
+      </c>
+      <c r="BA158">
+        <v>170</v>
+      </c>
+      <c r="BC158">
+        <v>60</v>
+      </c>
+      <c r="BD158">
+        <v>7</v>
+      </c>
+      <c r="BE158">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="159" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="H159">
+        <v>1</v>
+      </c>
+      <c r="I159">
+        <v>4</v>
+      </c>
+      <c r="AA159">
+        <v>2</v>
+      </c>
+      <c r="AB159">
+        <v>1</v>
+      </c>
+      <c r="AD159">
+        <v>1</v>
+      </c>
+      <c r="AE159">
+        <v>2</v>
+      </c>
+      <c r="AO159">
+        <v>1</v>
+      </c>
+      <c r="AQ159">
+        <v>2</v>
+      </c>
+      <c r="AR159">
+        <v>2</v>
+      </c>
+      <c r="AS159">
+        <v>2</v>
+      </c>
+      <c r="AV159">
+        <v>2</v>
+      </c>
+      <c r="AZ159">
+        <v>6</v>
+      </c>
+      <c r="BA159">
+        <v>5</v>
+      </c>
+      <c r="BC159">
+        <v>1</v>
+      </c>
+      <c r="BD159">
+        <v>3</v>
+      </c>
+      <c r="BE159">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:57" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+      <c r="I160" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AR160" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AS160" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AV160" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="161" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="B161" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I161">
+        <v>-7</v>
+      </c>
+      <c r="AA161">
+        <v>-13</v>
+      </c>
+      <c r="AR161">
+        <v>15</v>
+      </c>
+      <c r="AS161">
+        <v>100</v>
+      </c>
+      <c r="AV161">
+        <v>-9</v>
+      </c>
+      <c r="AZ161">
+        <v>-40</v>
+      </c>
+      <c r="BA161">
+        <v>185</v>
+      </c>
+      <c r="BD161">
+        <v>-23</v>
+      </c>
+      <c r="BE161">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="162" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="I162">
+        <v>1</v>
+      </c>
+      <c r="AA162">
+        <v>1</v>
+      </c>
+      <c r="AR162">
+        <v>2</v>
+      </c>
+      <c r="AS162">
+        <v>1</v>
+      </c>
+      <c r="AV162">
+        <v>1</v>
+      </c>
+      <c r="AZ162">
+        <v>4</v>
+      </c>
+      <c r="BA162">
+        <v>3</v>
+      </c>
+      <c r="BD162">
+        <v>2</v>
+      </c>
+      <c r="BE162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:57" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A164" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B164" s="1">
+        <v>16</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D164" s="1">
+        <v>10</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F164" s="1">
+        <v>500</v>
+      </c>
+      <c r="G164" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H164" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="B165">
+        <v>9</v>
+      </c>
+      <c r="E165" t="s">
+        <v>112</v>
+      </c>
+      <c r="F165">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="167" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="D167">
+        <v>20170807</v>
+      </c>
+      <c r="E167">
+        <v>20170808</v>
+      </c>
+      <c r="F167">
+        <v>20170809</v>
+      </c>
+      <c r="G167">
+        <v>20170810</v>
+      </c>
+      <c r="H167">
+        <v>20170811</v>
+      </c>
+      <c r="I167">
+        <v>20170814</v>
+      </c>
+      <c r="J167">
+        <v>20170815</v>
+      </c>
+      <c r="K167">
+        <v>20170816</v>
+      </c>
+      <c r="L167">
+        <v>20170817</v>
+      </c>
+      <c r="M167">
+        <v>20170818</v>
+      </c>
+      <c r="N167">
+        <v>20170821</v>
+      </c>
+      <c r="O167">
+        <v>20170822</v>
+      </c>
+      <c r="P167">
+        <v>20170823</v>
+      </c>
+      <c r="Q167">
+        <v>20170824</v>
+      </c>
+      <c r="R167">
+        <v>20170825</v>
+      </c>
+      <c r="S167">
+        <v>20170828</v>
+      </c>
+      <c r="T167">
+        <v>20170829</v>
+      </c>
+      <c r="U167">
+        <v>20170830</v>
+      </c>
+      <c r="V167">
+        <v>20170831</v>
+      </c>
+      <c r="W167">
+        <v>20170901</v>
+      </c>
+      <c r="X167">
+        <v>20170904</v>
+      </c>
+      <c r="Y167">
+        <v>20170905</v>
+      </c>
+      <c r="Z167">
+        <v>20170906</v>
+      </c>
+      <c r="AA167">
+        <v>20170907</v>
+      </c>
+      <c r="AB167">
+        <v>20170908</v>
+      </c>
+      <c r="AC167">
+        <v>20170911</v>
+      </c>
+      <c r="AD167">
+        <v>20170912</v>
+      </c>
+      <c r="AE167">
+        <v>20170913</v>
+      </c>
+      <c r="AF167">
+        <v>20170914</v>
+      </c>
+      <c r="AG167">
+        <v>20170915</v>
+      </c>
+      <c r="AH167">
+        <v>20170918</v>
+      </c>
+      <c r="AI167">
+        <v>20170919</v>
+      </c>
+      <c r="AJ167">
+        <v>20170920</v>
+      </c>
+      <c r="AK167">
+        <v>20170921</v>
+      </c>
+      <c r="AL167">
+        <v>20170922</v>
+      </c>
+      <c r="AM167">
+        <v>20170925</v>
+      </c>
+      <c r="AN167">
+        <v>20170926</v>
+      </c>
+      <c r="AO167">
+        <v>20170927</v>
+      </c>
+      <c r="AP167">
+        <v>20170928</v>
+      </c>
+      <c r="AQ167">
+        <v>20170929</v>
+      </c>
+      <c r="AR167">
+        <v>20171009</v>
+      </c>
+      <c r="AS167">
+        <v>20171010</v>
+      </c>
+      <c r="AT167">
+        <v>20171011</v>
+      </c>
+      <c r="AU167">
+        <v>20171012</v>
+      </c>
+      <c r="AV167">
+        <v>20171013</v>
+      </c>
+      <c r="AW167">
+        <v>20171016</v>
+      </c>
+      <c r="AX167">
+        <v>20171017</v>
+      </c>
+      <c r="AY167">
+        <v>20171018</v>
+      </c>
+      <c r="AZ167">
+        <v>20171019</v>
+      </c>
+      <c r="BA167">
+        <v>20171020</v>
+      </c>
+      <c r="BB167">
+        <v>20171023</v>
+      </c>
+      <c r="BC167">
+        <v>20171024</v>
+      </c>
+      <c r="BD167">
+        <v>20171025</v>
+      </c>
+      <c r="BE167">
+        <v>20171026</v>
+      </c>
+    </row>
+    <row r="168" spans="1:57" ht="27" x14ac:dyDescent="0.15">
+      <c r="A168" t="s">
+        <v>113</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H168">
+        <v>65</v>
+      </c>
+      <c r="I168">
+        <v>-5</v>
+      </c>
+      <c r="J168">
+        <v>70</v>
+      </c>
+      <c r="L168">
+        <v>-95</v>
+      </c>
+      <c r="M168">
+        <v>190</v>
+      </c>
+      <c r="P168">
+        <v>-85</v>
+      </c>
+      <c r="Q168">
+        <v>15</v>
+      </c>
+      <c r="U168">
+        <v>100</v>
+      </c>
+      <c r="AA168">
+        <v>-20</v>
+      </c>
+      <c r="AB168">
+        <v>-40</v>
+      </c>
+      <c r="AC168">
+        <v>5</v>
+      </c>
+      <c r="AD168">
+        <v>-95</v>
+      </c>
+      <c r="AE168">
+        <v>190</v>
+      </c>
+      <c r="AW168">
+        <v>-30</v>
+      </c>
+      <c r="AY168">
+        <v>25</v>
+      </c>
+      <c r="BA168">
+        <v>-5</v>
+      </c>
+      <c r="BB168">
+        <v>-65</v>
+      </c>
+      <c r="BC168">
+        <v>-20</v>
+      </c>
+      <c r="BD168">
+        <v>-5</v>
+      </c>
+      <c r="BE168">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="H169">
+        <v>1</v>
+      </c>
+      <c r="I169">
+        <v>1</v>
+      </c>
+      <c r="J169">
+        <v>1</v>
+      </c>
+      <c r="L169">
+        <v>5</v>
+      </c>
+      <c r="M169">
+        <v>1</v>
+      </c>
+      <c r="P169">
+        <v>5</v>
+      </c>
+      <c r="Q169">
+        <v>1</v>
+      </c>
+      <c r="U169">
+        <v>1</v>
+      </c>
+      <c r="AA169">
+        <v>3</v>
+      </c>
+      <c r="AB169">
+        <v>5</v>
+      </c>
+      <c r="AC169">
+        <v>1</v>
+      </c>
+      <c r="AD169">
+        <v>5</v>
+      </c>
+      <c r="AE169">
+        <v>4</v>
+      </c>
+      <c r="AW169">
+        <v>1</v>
+      </c>
+      <c r="AY169">
+        <v>2</v>
+      </c>
+      <c r="BA169">
+        <v>3</v>
+      </c>
+      <c r="BB169">
+        <v>4</v>
+      </c>
+      <c r="BC169">
+        <v>1</v>
+      </c>
+      <c r="BD169">
+        <v>2</v>
+      </c>
+      <c r="BE169">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="170" spans="1:57" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="B170" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H170" s="1">
+        <v>65</v>
+      </c>
+      <c r="I170" s="1">
+        <v>5</v>
+      </c>
+      <c r="J170" s="1">
+        <v>65</v>
+      </c>
+      <c r="L170" s="1">
+        <v>-65</v>
+      </c>
+      <c r="M170" s="1">
+        <v>195</v>
+      </c>
+      <c r="P170" s="1">
+        <v>-60</v>
+      </c>
+      <c r="Q170" s="1">
+        <v>5</v>
+      </c>
+      <c r="U170" s="1">
+        <v>85</v>
+      </c>
+      <c r="AA170" s="1">
+        <v>10</v>
+      </c>
+      <c r="AB170" s="1">
+        <v>-40</v>
+      </c>
+      <c r="AC170" s="1">
+        <v>10</v>
+      </c>
+      <c r="AD170" s="1">
+        <v>-65</v>
+      </c>
+      <c r="AE170" s="1">
+        <v>200</v>
+      </c>
+      <c r="AW170" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="171" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H171" s="1">
+        <v>1</v>
+      </c>
+      <c r="I171" s="1">
+        <v>1</v>
+      </c>
+      <c r="J171" s="1">
+        <v>1</v>
+      </c>
+      <c r="L171" s="1">
+        <v>4</v>
+      </c>
+      <c r="M171" s="1">
+        <v>1</v>
+      </c>
+      <c r="P171" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q171" s="1">
+        <v>1</v>
+      </c>
+      <c r="U171" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA171" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB171" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC171" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD171" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE171" s="1">
+        <v>4</v>
+      </c>
+      <c r="AW171" s="1">
+        <v>155</v>
+      </c>
+      <c r="AY171" s="1">
+        <v>50</v>
+      </c>
+      <c r="BA171" s="1">
+        <v>-35</v>
+      </c>
+      <c r="BB171" s="1">
+        <v>-65</v>
+      </c>
+      <c r="BC171" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD171" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE171" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="172" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="AW172">
+        <v>1</v>
+      </c>
+      <c r="AY172">
+        <v>1</v>
+      </c>
+      <c r="BA172">
+        <v>4</v>
+      </c>
+      <c r="BB172">
+        <v>4</v>
+      </c>
+      <c r="BC172">
+        <v>1</v>
+      </c>
+      <c r="BD172">
+        <v>2</v>
+      </c>
+      <c r="BE172">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:57" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A173" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B173" s="1">
+        <v>20</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D173" s="1">
+        <v>9</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F173" s="1">
+        <v>40</v>
+      </c>
+      <c r="G173" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H173" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:57" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="B174">
+        <v>20</v>
+      </c>
+      <c r="D174">
+        <v>14</v>
+      </c>
+      <c r="E174" t="s">
+        <v>112</v>
+      </c>
+      <c r="F174">
+        <v>100</v>
+      </c>
+      <c r="G174" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H174" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="D177">
+        <v>20170807</v>
+      </c>
+      <c r="E177">
+        <v>20170808</v>
+      </c>
+      <c r="F177">
+        <v>20170809</v>
+      </c>
+      <c r="G177">
+        <v>20170810</v>
+      </c>
+      <c r="H177">
+        <v>20170811</v>
+      </c>
+      <c r="I177">
+        <v>20170814</v>
+      </c>
+      <c r="J177">
+        <v>20170815</v>
+      </c>
+      <c r="K177">
+        <v>20170816</v>
+      </c>
+      <c r="L177">
+        <v>20170817</v>
+      </c>
+      <c r="M177">
+        <v>20170818</v>
+      </c>
+      <c r="N177">
+        <v>20170821</v>
+      </c>
+      <c r="O177">
+        <v>20170822</v>
+      </c>
+      <c r="P177">
+        <v>20170823</v>
+      </c>
+      <c r="Q177">
+        <v>20170824</v>
+      </c>
+      <c r="R177">
+        <v>20170825</v>
+      </c>
+      <c r="S177">
+        <v>20170828</v>
+      </c>
+      <c r="T177">
+        <v>20170829</v>
+      </c>
+      <c r="U177">
+        <v>20170830</v>
+      </c>
+      <c r="V177">
+        <v>20170831</v>
+      </c>
+      <c r="W177">
+        <v>20170901</v>
+      </c>
+      <c r="X177">
+        <v>20170904</v>
+      </c>
+      <c r="Y177">
+        <v>20170905</v>
+      </c>
+      <c r="Z177">
+        <v>20170906</v>
+      </c>
+      <c r="AA177">
+        <v>20170907</v>
+      </c>
+      <c r="AB177">
+        <v>20170908</v>
+      </c>
+      <c r="AC177">
+        <v>20170911</v>
+      </c>
+      <c r="AD177">
+        <v>20170912</v>
+      </c>
+      <c r="AE177">
+        <v>20170913</v>
+      </c>
+      <c r="AF177">
+        <v>20170914</v>
+      </c>
+      <c r="AG177">
+        <v>20170915</v>
+      </c>
+      <c r="AH177">
+        <v>20170918</v>
+      </c>
+      <c r="AI177">
+        <v>20170919</v>
+      </c>
+      <c r="AJ177">
+        <v>20170920</v>
+      </c>
+      <c r="AK177">
+        <v>20170921</v>
+      </c>
+      <c r="AL177">
+        <v>20170922</v>
+      </c>
+      <c r="AM177">
+        <v>20170925</v>
+      </c>
+      <c r="AN177">
+        <v>20170926</v>
+      </c>
+      <c r="AO177">
+        <v>20170927</v>
+      </c>
+      <c r="AP177">
+        <v>20170928</v>
+      </c>
+      <c r="AQ177">
+        <v>20170929</v>
+      </c>
+      <c r="AR177">
+        <v>20171009</v>
+      </c>
+      <c r="AS177">
+        <v>20171010</v>
+      </c>
+      <c r="AT177">
+        <v>20171011</v>
+      </c>
+      <c r="AU177">
+        <v>20171012</v>
+      </c>
+      <c r="AV177">
+        <v>20171013</v>
+      </c>
+      <c r="AW177">
+        <v>20171016</v>
+      </c>
+      <c r="AX177">
+        <v>20171017</v>
+      </c>
+      <c r="AY177">
+        <v>20171018</v>
+      </c>
+      <c r="AZ177">
+        <v>20171019</v>
+      </c>
+      <c r="BA177">
+        <v>20171020</v>
+      </c>
+      <c r="BB177">
+        <v>20171023</v>
+      </c>
+      <c r="BC177">
+        <v>20171024</v>
+      </c>
+      <c r="BD177">
+        <v>20171025</v>
+      </c>
+      <c r="BE177">
+        <v>20171026</v>
+      </c>
+    </row>
+    <row r="178" spans="1:57" ht="27" x14ac:dyDescent="0.15">
+      <c r="A178" t="s">
+        <v>117</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E178">
+        <v>34</v>
+      </c>
+      <c r="F178">
+        <v>32</v>
+      </c>
+      <c r="G178">
+        <v>58</v>
+      </c>
+      <c r="H178">
+        <v>-52</v>
+      </c>
+      <c r="I178">
+        <v>-4</v>
+      </c>
+      <c r="J178">
+        <v>-36</v>
+      </c>
+      <c r="M178">
+        <v>-6</v>
+      </c>
+      <c r="N178">
+        <v>10</v>
+      </c>
+      <c r="R178">
+        <v>-36</v>
+      </c>
+      <c r="S178">
+        <v>2</v>
+      </c>
+      <c r="T178">
+        <v>34</v>
+      </c>
+      <c r="U178">
+        <v>30</v>
+      </c>
+      <c r="V178">
+        <v>-2</v>
+      </c>
+      <c r="W178">
+        <v>-4</v>
+      </c>
+      <c r="Y178">
+        <v>20</v>
+      </c>
+      <c r="Z178">
+        <v>4</v>
+      </c>
+      <c r="AA178">
+        <v>0</v>
+      </c>
+      <c r="AB178">
+        <v>10</v>
+      </c>
+      <c r="AC178">
+        <v>-8</v>
+      </c>
+      <c r="AD178">
+        <v>-8</v>
+      </c>
+      <c r="AE178">
+        <v>-56</v>
+      </c>
+      <c r="AF178">
+        <v>34</v>
+      </c>
+      <c r="AG178">
+        <v>10</v>
+      </c>
+      <c r="AH178">
+        <v>-24</v>
+      </c>
+      <c r="AI178">
+        <v>14</v>
+      </c>
+      <c r="AJ178">
+        <v>-16</v>
+      </c>
+      <c r="AK178">
+        <v>48</v>
+      </c>
+      <c r="AR178">
+        <v>6</v>
+      </c>
+      <c r="AU178">
+        <v>-12</v>
+      </c>
+      <c r="AV178">
+        <v>-38</v>
+      </c>
+      <c r="AW178">
+        <v>-28</v>
+      </c>
+      <c r="AX178">
+        <v>2</v>
+      </c>
+      <c r="AY178">
+        <v>16</v>
+      </c>
+      <c r="AZ178">
+        <v>64</v>
+      </c>
+      <c r="BA178">
+        <v>-24</v>
+      </c>
+      <c r="BB178">
+        <v>-50</v>
+      </c>
+      <c r="BC178">
+        <v>-22</v>
+      </c>
+      <c r="BD178">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="179" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="B179" s="1"/>
+      <c r="E179">
+        <v>3</v>
+      </c>
+      <c r="F179">
+        <v>1</v>
+      </c>
+      <c r="G179">
+        <v>2</v>
+      </c>
+      <c r="H179">
+        <v>6</v>
+      </c>
+      <c r="I179">
+        <v>4</v>
+      </c>
+      <c r="J179">
+        <v>5</v>
+      </c>
+      <c r="M179">
+        <v>5</v>
+      </c>
+      <c r="N179">
+        <v>2</v>
+      </c>
+      <c r="R179">
+        <v>3</v>
+      </c>
+      <c r="S179">
+        <v>1</v>
+      </c>
+      <c r="T179">
+        <v>1</v>
+      </c>
+      <c r="U179">
+        <v>1</v>
+      </c>
+      <c r="V179">
+        <v>2</v>
+      </c>
+      <c r="W179">
+        <v>2</v>
+      </c>
+      <c r="Y179">
+        <v>3</v>
+      </c>
+      <c r="Z179">
+        <v>2</v>
+      </c>
+      <c r="AA179">
+        <v>3</v>
+      </c>
+      <c r="AB179">
+        <v>4</v>
+      </c>
+      <c r="AC179">
+        <v>4</v>
+      </c>
+      <c r="AD179">
+        <v>2</v>
+      </c>
+      <c r="AE179">
+        <v>7</v>
+      </c>
+      <c r="AF179">
+        <v>1</v>
+      </c>
+      <c r="AG179">
+        <v>2</v>
+      </c>
+      <c r="AH179">
+        <v>3</v>
+      </c>
+      <c r="AI179">
+        <v>3</v>
+      </c>
+      <c r="AJ179">
+        <v>4</v>
+      </c>
+      <c r="AK179">
+        <v>2</v>
+      </c>
+      <c r="AR179">
+        <v>2</v>
+      </c>
+      <c r="AU179">
+        <v>1</v>
+      </c>
+      <c r="AV179">
+        <v>5</v>
+      </c>
+      <c r="AW179">
+        <v>4</v>
+      </c>
+      <c r="AX179">
+        <v>2</v>
+      </c>
+      <c r="AY179">
+        <v>1</v>
+      </c>
+      <c r="AZ179">
+        <v>1</v>
+      </c>
+      <c r="BA179">
+        <v>3</v>
+      </c>
+      <c r="BB179">
+        <v>6</v>
+      </c>
+      <c r="BC179">
+        <v>3</v>
+      </c>
+      <c r="BD179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="B180" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E180">
+        <v>44</v>
+      </c>
+      <c r="F180">
+        <v>32</v>
+      </c>
+      <c r="G180">
+        <v>56</v>
+      </c>
+      <c r="H180">
+        <v>-52</v>
+      </c>
+      <c r="I180">
+        <v>-4</v>
+      </c>
+      <c r="J180">
+        <v>-12</v>
+      </c>
+      <c r="M180">
+        <v>20</v>
+      </c>
+      <c r="N180">
+        <v>10</v>
+      </c>
+      <c r="R180">
+        <v>-36</v>
+      </c>
+      <c r="S180">
+        <v>-4</v>
+      </c>
+      <c r="T180">
+        <v>34</v>
+      </c>
+      <c r="U180">
+        <v>32</v>
+      </c>
+      <c r="V180">
+        <v>4</v>
+      </c>
+      <c r="W180">
+        <v>-28</v>
+      </c>
+      <c r="Y180">
+        <v>20</v>
+      </c>
+      <c r="Z180">
+        <v>14</v>
+      </c>
+      <c r="AA180">
+        <v>0</v>
+      </c>
+      <c r="AC180">
+        <v>10</v>
+      </c>
+      <c r="AD180">
+        <v>-24</v>
+      </c>
+      <c r="AE180">
+        <v>-66</v>
+      </c>
+      <c r="AF180">
+        <v>32</v>
+      </c>
+      <c r="AG180">
+        <v>18</v>
+      </c>
+      <c r="AH180">
+        <v>-22</v>
+      </c>
+      <c r="AI180">
+        <v>14</v>
+      </c>
+      <c r="AJ180">
+        <v>-26</v>
+      </c>
+      <c r="AK180">
+        <v>58</v>
+      </c>
+      <c r="AR180">
+        <v>20</v>
+      </c>
+      <c r="AU180">
+        <v>-12</v>
+      </c>
+      <c r="AV180">
+        <v>-38</v>
+      </c>
+      <c r="AW180">
+        <v>-32</v>
+      </c>
+      <c r="AX180">
+        <v>2</v>
+      </c>
+      <c r="AY180">
+        <v>6</v>
+      </c>
+      <c r="AZ180">
+        <v>64</v>
+      </c>
+      <c r="BA180">
+        <v>-12</v>
+      </c>
+      <c r="BB180">
+        <v>-26</v>
+      </c>
+      <c r="BC180">
+        <v>-26</v>
+      </c>
+      <c r="BD180">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="181" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="E181">
+        <v>2</v>
+      </c>
+      <c r="F181">
+        <v>1</v>
+      </c>
+      <c r="G181">
+        <v>2</v>
+      </c>
+      <c r="H181">
+        <v>5</v>
+      </c>
+      <c r="I181">
+        <v>4</v>
+      </c>
+      <c r="J181">
+        <v>3</v>
+      </c>
+      <c r="M181">
+        <v>3</v>
+      </c>
+      <c r="N181">
+        <v>1</v>
+      </c>
+      <c r="R181">
+        <v>3</v>
+      </c>
+      <c r="S181">
+        <v>1</v>
+      </c>
+      <c r="T181">
+        <v>1</v>
+      </c>
+      <c r="U181">
+        <v>2</v>
+      </c>
+      <c r="V181">
+        <v>2</v>
+      </c>
+      <c r="W181">
+        <v>4</v>
+      </c>
+      <c r="Y181">
+        <v>3</v>
+      </c>
+      <c r="Z181">
+        <v>1</v>
+      </c>
+      <c r="AA181">
+        <v>3</v>
+      </c>
+      <c r="AC181" s="3">
+        <v>4</v>
+      </c>
+      <c r="AD181">
+        <v>3</v>
+      </c>
+      <c r="AE181">
+        <v>7</v>
+      </c>
+      <c r="AF181">
+        <v>1</v>
+      </c>
+      <c r="AG181">
+        <v>1</v>
+      </c>
+      <c r="AH181">
+        <v>3</v>
+      </c>
+      <c r="AI181">
+        <v>3</v>
+      </c>
+      <c r="AJ181">
+        <v>4</v>
+      </c>
+      <c r="AK181">
+        <v>1</v>
+      </c>
+      <c r="AR181">
+        <v>1</v>
+      </c>
+      <c r="AU181">
+        <v>1</v>
+      </c>
+      <c r="AV181">
+        <v>5</v>
+      </c>
+      <c r="AW181">
+        <v>4</v>
+      </c>
+      <c r="AX181">
+        <v>2</v>
+      </c>
+      <c r="AY181">
+        <v>2</v>
+      </c>
+      <c r="AZ181">
+        <v>1</v>
+      </c>
+      <c r="BA181">
+        <v>2</v>
+      </c>
+      <c r="BB181">
+        <v>4</v>
+      </c>
+      <c r="BC181">
+        <v>3</v>
+      </c>
+      <c r="BD181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:57" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="B183" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E183">
+        <v>34</v>
+      </c>
+      <c r="F183">
+        <v>32</v>
+      </c>
+      <c r="G183">
+        <v>54</v>
+      </c>
+      <c r="H183">
+        <v>-62</v>
+      </c>
+      <c r="I183">
+        <v>-6</v>
+      </c>
+      <c r="J183">
+        <v>-36</v>
+      </c>
+      <c r="M183">
+        <v>16</v>
+      </c>
+      <c r="N183">
+        <v>10</v>
+      </c>
+      <c r="R183">
+        <v>-36</v>
+      </c>
+      <c r="T183">
+        <v>34</v>
+      </c>
+      <c r="U183">
+        <v>22</v>
+      </c>
+      <c r="V183">
+        <v>8</v>
+      </c>
+      <c r="W183">
+        <v>0</v>
+      </c>
+      <c r="Y183">
+        <v>8</v>
+      </c>
+      <c r="Z183">
+        <v>8</v>
+      </c>
+      <c r="AA183">
+        <v>-10</v>
+      </c>
+      <c r="AB183">
+        <v>2</v>
+      </c>
+      <c r="AC183">
+        <v>-20</v>
+      </c>
+      <c r="AD183">
+        <v>-18</v>
+      </c>
+      <c r="AE183">
+        <v>-58</v>
+      </c>
+      <c r="AF183">
+        <v>34</v>
+      </c>
+      <c r="AG183">
+        <v>12</v>
+      </c>
+      <c r="AH183">
+        <v>-12</v>
+      </c>
+      <c r="AI183">
+        <v>4</v>
+      </c>
+      <c r="AJ183">
+        <v>-14</v>
+      </c>
+      <c r="AK183">
+        <v>54</v>
+      </c>
+      <c r="AR183">
+        <v>20</v>
+      </c>
+      <c r="AU183">
+        <v>-2</v>
+      </c>
+      <c r="AV183">
+        <v>-46</v>
+      </c>
+      <c r="AW183">
+        <v>-26</v>
+      </c>
+      <c r="AX183">
+        <v>0</v>
+      </c>
+      <c r="AY183">
+        <v>16</v>
+      </c>
+      <c r="AZ183">
+        <v>64</v>
+      </c>
+      <c r="BA183">
+        <v>-22</v>
+      </c>
+      <c r="BB183">
+        <v>-36</v>
+      </c>
+      <c r="BC183">
+        <v>-26</v>
+      </c>
+      <c r="BD183">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="184" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="E184">
+        <v>3</v>
+      </c>
+      <c r="F184">
+        <v>1</v>
+      </c>
+      <c r="G184">
+        <v>2</v>
+      </c>
+      <c r="H184">
+        <v>6</v>
+      </c>
+      <c r="I184">
+        <v>3</v>
+      </c>
+      <c r="J184">
+        <v>4</v>
+      </c>
+      <c r="M184">
+        <v>3</v>
+      </c>
+      <c r="N184">
+        <v>1</v>
+      </c>
+      <c r="R184">
+        <v>2</v>
+      </c>
+      <c r="T184">
+        <v>1</v>
+      </c>
+      <c r="U184">
+        <v>1</v>
+      </c>
+      <c r="V184">
+        <v>1</v>
+      </c>
+      <c r="W184">
+        <v>1</v>
+      </c>
+      <c r="Y184">
+        <v>2</v>
+      </c>
+      <c r="Z184">
+        <v>1</v>
+      </c>
+      <c r="AA184">
+        <v>3</v>
+      </c>
+      <c r="AB184">
+        <v>4</v>
+      </c>
+      <c r="AC184">
+        <v>3</v>
+      </c>
+      <c r="AD184">
+        <v>2</v>
+      </c>
+      <c r="AE184">
+        <v>6</v>
+      </c>
+      <c r="AF184">
+        <v>1</v>
+      </c>
+      <c r="AG184">
+        <v>1</v>
+      </c>
+      <c r="AH184">
+        <v>2</v>
+      </c>
+      <c r="AI184">
+        <v>3</v>
+      </c>
+      <c r="AJ184">
+        <v>3</v>
+      </c>
+      <c r="AK184">
+        <v>1</v>
+      </c>
+      <c r="AR184">
+        <v>1</v>
+      </c>
+      <c r="AU184">
+        <v>1</v>
+      </c>
+      <c r="AV184">
+        <v>4</v>
+      </c>
+      <c r="AW184">
+        <v>2</v>
+      </c>
+      <c r="AX184">
+        <v>2</v>
+      </c>
+      <c r="AY184">
+        <v>1</v>
+      </c>
+      <c r="AZ184">
+        <v>1</v>
+      </c>
+      <c r="BA184">
+        <v>2</v>
+      </c>
+      <c r="BB184">
+        <v>3</v>
+      </c>
+      <c r="BC184">
+        <v>3</v>
+      </c>
+      <c r="BD184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:57" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A186" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B186" s="1">
+        <v>37</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D186" s="1">
+        <v>20</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F186" s="1">
+        <v>0</v>
+      </c>
+      <c r="G186" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H186" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:57" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="B187">
+        <v>20</v>
+      </c>
+      <c r="D187">
+        <v>14</v>
+      </c>
+      <c r="E187" t="s">
+        <v>112</v>
+      </c>
+      <c r="F187">
+        <v>75</v>
+      </c>
+      <c r="G187" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H187" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:57" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="A189" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F189">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="192" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="D192">
+        <v>20170807</v>
+      </c>
+      <c r="E192">
+        <v>20170808</v>
+      </c>
+      <c r="F192">
+        <v>20170809</v>
+      </c>
+      <c r="G192">
+        <v>20170810</v>
+      </c>
+      <c r="H192">
+        <v>20170811</v>
+      </c>
+      <c r="I192">
+        <v>20170814</v>
+      </c>
+      <c r="J192">
+        <v>20170815</v>
+      </c>
+      <c r="K192">
+        <v>20170816</v>
+      </c>
+      <c r="L192">
+        <v>20170817</v>
+      </c>
+      <c r="M192">
+        <v>20170818</v>
+      </c>
+      <c r="N192">
+        <v>20170821</v>
+      </c>
+      <c r="O192">
+        <v>20170822</v>
+      </c>
+      <c r="P192">
+        <v>20170823</v>
+      </c>
+      <c r="Q192">
+        <v>20170824</v>
+      </c>
+      <c r="R192">
+        <v>20170825</v>
+      </c>
+      <c r="S192">
+        <v>20170828</v>
+      </c>
+      <c r="T192">
+        <v>20170829</v>
+      </c>
+      <c r="U192">
+        <v>20170830</v>
+      </c>
+      <c r="V192">
+        <v>20170831</v>
+      </c>
+      <c r="W192">
+        <v>20170901</v>
+      </c>
+      <c r="X192">
+        <v>20170904</v>
+      </c>
+      <c r="Y192">
+        <v>20170905</v>
+      </c>
+      <c r="Z192">
+        <v>20170906</v>
+      </c>
+      <c r="AA192">
+        <v>20170907</v>
+      </c>
+      <c r="AB192">
+        <v>20170908</v>
+      </c>
+      <c r="AC192">
+        <v>20170911</v>
+      </c>
+      <c r="AD192">
+        <v>20170912</v>
+      </c>
+      <c r="AE192">
+        <v>20170913</v>
+      </c>
+      <c r="AF192">
+        <v>20170914</v>
+      </c>
+      <c r="AG192">
+        <v>20170915</v>
+      </c>
+      <c r="AH192">
+        <v>20170918</v>
+      </c>
+      <c r="AI192">
+        <v>20170919</v>
+      </c>
+      <c r="AJ192">
+        <v>20170920</v>
+      </c>
+      <c r="AK192">
+        <v>20170921</v>
+      </c>
+      <c r="AL192">
+        <v>20170922</v>
+      </c>
+      <c r="AM192">
+        <v>20170925</v>
+      </c>
+      <c r="AN192">
+        <v>20170926</v>
+      </c>
+      <c r="AO192">
+        <v>20170927</v>
+      </c>
+      <c r="AP192">
+        <v>20170928</v>
+      </c>
+      <c r="AQ192">
+        <v>20170929</v>
+      </c>
+      <c r="AR192">
+        <v>20171009</v>
+      </c>
+      <c r="AS192">
+        <v>20171010</v>
+      </c>
+      <c r="AT192">
+        <v>20171011</v>
+      </c>
+      <c r="AU192">
+        <v>20171012</v>
+      </c>
+      <c r="AV192">
+        <v>20171013</v>
+      </c>
+      <c r="AW192">
+        <v>20171016</v>
+      </c>
+      <c r="AX192">
+        <v>20171017</v>
+      </c>
+      <c r="AY192">
+        <v>20171018</v>
+      </c>
+      <c r="AZ192">
+        <v>20171019</v>
+      </c>
+      <c r="BA192">
+        <v>20171020</v>
+      </c>
+      <c r="BB192">
+        <v>20171023</v>
+      </c>
+      <c r="BC192">
+        <v>20171024</v>
+      </c>
+      <c r="BD192">
+        <v>20171025</v>
+      </c>
+      <c r="BE192">
+        <v>20171026</v>
+      </c>
+    </row>
+    <row r="193" spans="1:57" ht="27" x14ac:dyDescent="0.15">
+      <c r="A193" t="s">
+        <v>116</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D193">
+        <v>58</v>
+      </c>
+      <c r="E193">
+        <v>-30</v>
+      </c>
+      <c r="F193">
+        <v>24</v>
+      </c>
+      <c r="G193">
+        <v>-24</v>
+      </c>
+      <c r="H193">
+        <v>6</v>
+      </c>
+      <c r="I193">
+        <v>46</v>
+      </c>
+      <c r="J193">
+        <v>-34</v>
+      </c>
+      <c r="M193">
+        <v>14</v>
+      </c>
+      <c r="R193">
+        <v>-4</v>
+      </c>
+      <c r="S193">
+        <v>10</v>
+      </c>
+      <c r="T193">
+        <v>12</v>
+      </c>
+      <c r="U193">
+        <v>-12</v>
+      </c>
+      <c r="V193">
+        <v>6</v>
+      </c>
+      <c r="W193">
+        <v>8</v>
+      </c>
+      <c r="X193">
+        <v>-4</v>
+      </c>
+      <c r="Y193">
+        <v>26</v>
+      </c>
+      <c r="Z193">
+        <v>18</v>
+      </c>
+      <c r="AA193">
+        <v>-14</v>
+      </c>
+      <c r="AB193">
+        <v>-32</v>
+      </c>
+      <c r="AC193">
+        <v>58</v>
+      </c>
+      <c r="AH193">
+        <v>16</v>
+      </c>
+      <c r="AI193">
+        <v>28</v>
+      </c>
+      <c r="AJ193">
+        <v>-8</v>
+      </c>
+      <c r="AK193">
+        <v>8</v>
+      </c>
+      <c r="AN193">
+        <v>12</v>
+      </c>
+      <c r="AO193">
+        <v>-24</v>
+      </c>
+      <c r="AR193">
+        <v>-60</v>
+      </c>
+      <c r="AS193">
+        <v>22</v>
+      </c>
+      <c r="AT193">
+        <v>16</v>
+      </c>
+      <c r="AU193">
+        <v>-48</v>
+      </c>
+      <c r="AV193">
+        <v>24</v>
+      </c>
+      <c r="AW193">
+        <v>-18</v>
+      </c>
+      <c r="AX193">
+        <v>34</v>
+      </c>
+      <c r="AY193">
+        <v>-8</v>
+      </c>
+      <c r="AZ193">
+        <v>52</v>
+      </c>
+      <c r="BA193">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="194" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="D194">
+        <v>1</v>
+      </c>
+      <c r="E194">
+        <v>4</v>
+      </c>
+      <c r="F194">
+        <v>1</v>
+      </c>
+      <c r="G194">
+        <v>3</v>
+      </c>
+      <c r="H194">
+        <v>3</v>
+      </c>
+      <c r="I194">
+        <v>2</v>
+      </c>
+      <c r="J194">
+        <v>5</v>
+      </c>
+      <c r="M194">
+        <v>3</v>
+      </c>
+      <c r="R194">
+        <v>2</v>
+      </c>
+      <c r="S194">
+        <v>1</v>
+      </c>
+      <c r="T194">
+        <v>2</v>
+      </c>
+      <c r="U194">
+        <v>4</v>
+      </c>
+      <c r="V194">
+        <v>1</v>
+      </c>
+      <c r="W194">
+        <v>1</v>
+      </c>
+      <c r="X194">
+        <v>1</v>
+      </c>
+      <c r="Y194">
+        <v>3</v>
+      </c>
+      <c r="Z194">
+        <v>1</v>
+      </c>
+      <c r="AA194">
+        <v>3</v>
+      </c>
+      <c r="AB194">
+        <v>5</v>
+      </c>
+      <c r="AC194">
+        <v>3</v>
+      </c>
+      <c r="AH194">
+        <v>1</v>
+      </c>
+      <c r="AI194">
+        <v>1</v>
+      </c>
+      <c r="AJ194">
+        <v>2</v>
+      </c>
+      <c r="AK194">
+        <v>4</v>
+      </c>
+      <c r="AN194">
+        <v>1</v>
+      </c>
+      <c r="AO194">
+        <v>3</v>
+      </c>
+      <c r="AR194">
+        <v>4</v>
+      </c>
+      <c r="AS194">
+        <v>1</v>
+      </c>
+      <c r="AT194">
+        <v>1</v>
+      </c>
+      <c r="AU194">
+        <v>4</v>
+      </c>
+      <c r="AV194">
+        <v>3</v>
+      </c>
+      <c r="AW194">
+        <v>3</v>
+      </c>
+      <c r="AX194">
+        <v>1</v>
+      </c>
+      <c r="AY194">
+        <v>3</v>
+      </c>
+      <c r="AZ194">
+        <v>2</v>
+      </c>
+      <c r="BA194">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B195" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D195" s="1">
+        <v>56</v>
+      </c>
+      <c r="E195" s="1">
+        <v>-32</v>
+      </c>
+      <c r="F195" s="1">
+        <v>14</v>
+      </c>
+      <c r="G195" s="1">
+        <v>-20</v>
+      </c>
+      <c r="H195" s="1">
+        <v>18</v>
+      </c>
+      <c r="I195" s="1">
+        <v>36</v>
+      </c>
+      <c r="J195" s="1">
+        <v>-30</v>
+      </c>
+      <c r="M195" s="1">
+        <v>24</v>
+      </c>
+      <c r="R195" s="1">
+        <v>-6</v>
+      </c>
+      <c r="S195" s="1">
+        <v>-2</v>
+      </c>
+      <c r="T195" s="1">
+        <v>20</v>
+      </c>
+      <c r="U195" s="1">
+        <v>-22</v>
+      </c>
+      <c r="V195" s="1">
+        <v>6</v>
+      </c>
+      <c r="W195" s="1">
+        <v>-10</v>
+      </c>
+      <c r="X195">
+        <v>-4</v>
+      </c>
+      <c r="Y195" s="1">
+        <v>16</v>
+      </c>
+      <c r="Z195" s="1">
+        <v>18</v>
+      </c>
+      <c r="AA195" s="1">
+        <v>-8</v>
+      </c>
+      <c r="AB195" s="1">
+        <v>-28</v>
+      </c>
+      <c r="AC195" s="1">
+        <v>62</v>
+      </c>
+      <c r="AH195" s="1">
+        <v>16</v>
+      </c>
+      <c r="AJ195" s="1">
+        <v>-12</v>
+      </c>
+      <c r="AK195" s="1">
+        <v>16</v>
+      </c>
+      <c r="AO195" s="1">
+        <v>-24</v>
+      </c>
+      <c r="AR195" s="1">
+        <v>-64</v>
+      </c>
+      <c r="AS195" s="1">
+        <v>22</v>
+      </c>
+      <c r="AT195" s="1">
+        <v>18</v>
+      </c>
+      <c r="AU195" s="1">
+        <v>-30</v>
+      </c>
+      <c r="AV195" s="1">
+        <v>16</v>
+      </c>
+      <c r="AW195" s="1">
+        <v>-24</v>
+      </c>
+      <c r="AX195" s="1">
+        <v>34</v>
+      </c>
+      <c r="AY195" s="1">
+        <v>-16</v>
+      </c>
+      <c r="AZ195" s="1">
+        <v>52</v>
+      </c>
+      <c r="BA195" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="196" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="D196">
+        <v>1</v>
+      </c>
+      <c r="E196">
+        <v>4</v>
+      </c>
+      <c r="F196">
+        <v>1</v>
+      </c>
+      <c r="G196">
+        <v>3</v>
+      </c>
+      <c r="H196">
+        <v>2</v>
+      </c>
+      <c r="I196">
+        <v>2</v>
+      </c>
+      <c r="J196">
+        <v>4</v>
+      </c>
+      <c r="M196">
+        <v>3</v>
+      </c>
+      <c r="R196">
+        <v>1</v>
+      </c>
+      <c r="S196">
+        <v>1</v>
+      </c>
+      <c r="T196">
+        <v>2</v>
+      </c>
+      <c r="U196">
+        <v>4</v>
+      </c>
+      <c r="V196">
+        <v>1</v>
+      </c>
+      <c r="W196">
+        <v>2</v>
+      </c>
+      <c r="X196">
+        <v>1</v>
+      </c>
+      <c r="Y196">
+        <v>3</v>
+      </c>
+      <c r="Z196">
+        <v>1</v>
+      </c>
+      <c r="AA196">
+        <v>3</v>
+      </c>
+      <c r="AB196">
+        <v>5</v>
+      </c>
+      <c r="AC196">
+        <v>3</v>
+      </c>
+      <c r="AH196">
+        <v>1</v>
+      </c>
+      <c r="AJ196">
+        <v>2</v>
+      </c>
+      <c r="AK196">
+        <v>4</v>
+      </c>
+      <c r="AO196">
+        <v>3</v>
+      </c>
+      <c r="AR196">
+        <v>5</v>
+      </c>
+      <c r="AS196">
+        <v>1</v>
+      </c>
+      <c r="AT196">
+        <v>1</v>
+      </c>
+      <c r="AU196">
+        <v>3</v>
+      </c>
+      <c r="AV196">
+        <v>3</v>
+      </c>
+      <c r="AW196">
+        <v>3</v>
+      </c>
+      <c r="AX196">
+        <v>1</v>
+      </c>
+      <c r="AY196">
+        <v>3</v>
+      </c>
+      <c r="AZ196">
+        <v>2</v>
+      </c>
+      <c r="BA196">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:57" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A198" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B198" s="1">
+        <v>36</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D198" s="1">
+        <v>22</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F198" s="1">
+        <v>90</v>
+      </c>
+      <c r="G198" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H198" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:57" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="B199">
+        <v>20</v>
+      </c>
+      <c r="D199">
+        <v>14</v>
+      </c>
+      <c r="E199" t="s">
+        <v>112</v>
+      </c>
+      <c r="F199">
+        <v>60</v>
+      </c>
+      <c r="G199" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H199" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="D202">
+        <v>20170807</v>
+      </c>
+      <c r="E202">
+        <v>20170808</v>
+      </c>
+      <c r="F202">
+        <v>20170809</v>
+      </c>
+      <c r="G202">
+        <v>20170810</v>
+      </c>
+      <c r="H202">
+        <v>20170811</v>
+      </c>
+      <c r="I202">
+        <v>20170814</v>
+      </c>
+      <c r="J202">
+        <v>20170815</v>
+      </c>
+      <c r="K202">
+        <v>20170816</v>
+      </c>
+      <c r="L202">
+        <v>20170817</v>
+      </c>
+      <c r="M202">
+        <v>20170818</v>
+      </c>
+      <c r="N202">
+        <v>20170821</v>
+      </c>
+      <c r="O202">
+        <v>20170822</v>
+      </c>
+      <c r="P202">
+        <v>20170823</v>
+      </c>
+      <c r="Q202">
+        <v>20170824</v>
+      </c>
+      <c r="R202">
+        <v>20170825</v>
+      </c>
+      <c r="S202">
+        <v>20170828</v>
+      </c>
+      <c r="T202">
+        <v>20170829</v>
+      </c>
+      <c r="U202">
+        <v>20170830</v>
+      </c>
+      <c r="V202">
+        <v>20170831</v>
+      </c>
+      <c r="W202">
+        <v>20170901</v>
+      </c>
+      <c r="X202">
+        <v>20170904</v>
+      </c>
+      <c r="Y202">
+        <v>20170905</v>
+      </c>
+      <c r="Z202">
+        <v>20170906</v>
+      </c>
+      <c r="AA202">
+        <v>20170907</v>
+      </c>
+      <c r="AB202">
+        <v>20170908</v>
+      </c>
+      <c r="AC202">
+        <v>20170911</v>
+      </c>
+      <c r="AD202">
+        <v>20170912</v>
+      </c>
+      <c r="AE202">
+        <v>20170913</v>
+      </c>
+      <c r="AF202">
+        <v>20170914</v>
+      </c>
+      <c r="AG202">
+        <v>20170915</v>
+      </c>
+      <c r="AH202">
+        <v>20170918</v>
+      </c>
+      <c r="AI202">
+        <v>20170919</v>
+      </c>
+      <c r="AJ202">
+        <v>20170920</v>
+      </c>
+      <c r="AK202">
+        <v>20170921</v>
+      </c>
+      <c r="AL202">
+        <v>20170922</v>
+      </c>
+      <c r="AM202">
+        <v>20170925</v>
+      </c>
+      <c r="AN202">
+        <v>20170926</v>
+      </c>
+      <c r="AO202">
+        <v>20170927</v>
+      </c>
+      <c r="AP202">
+        <v>20170928</v>
+      </c>
+      <c r="AQ202">
+        <v>20170929</v>
+      </c>
+      <c r="AR202">
+        <v>20171009</v>
+      </c>
+      <c r="AS202">
+        <v>20171010</v>
+      </c>
+      <c r="AT202">
+        <v>20171011</v>
+      </c>
+      <c r="AU202">
+        <v>20171012</v>
+      </c>
+      <c r="AV202">
+        <v>20171013</v>
+      </c>
+      <c r="AW202">
+        <v>20171016</v>
+      </c>
+      <c r="AX202">
+        <v>20171017</v>
+      </c>
+      <c r="AY202">
+        <v>20171018</v>
+      </c>
+      <c r="AZ202">
+        <v>20171019</v>
+      </c>
+      <c r="BA202">
+        <v>20171020</v>
+      </c>
+      <c r="BB202">
+        <v>20171023</v>
+      </c>
+      <c r="BC202">
+        <v>20171024</v>
+      </c>
+      <c r="BD202">
+        <v>20171025</v>
+      </c>
+      <c r="BE202">
+        <v>20171026</v>
+      </c>
+    </row>
+    <row r="203" spans="1:57" ht="27" x14ac:dyDescent="0.15">
+      <c r="A203" t="s">
+        <v>118</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D203">
+        <v>-5</v>
+      </c>
+      <c r="E203">
+        <v>2</v>
+      </c>
+      <c r="N203">
+        <v>1</v>
+      </c>
+      <c r="O203">
+        <v>16</v>
+      </c>
+      <c r="P203">
+        <v>-3</v>
+      </c>
+      <c r="Q203">
+        <v>1</v>
+      </c>
+      <c r="R203">
+        <v>-8</v>
+      </c>
+      <c r="S203">
+        <v>-3</v>
+      </c>
+      <c r="T203">
+        <v>16</v>
+      </c>
+      <c r="X203">
+        <v>-9</v>
+      </c>
+      <c r="Y203">
+        <v>5</v>
+      </c>
+      <c r="Z203">
+        <v>-4</v>
+      </c>
+      <c r="AA203">
+        <v>-1</v>
+      </c>
+      <c r="AB203">
+        <v>15</v>
+      </c>
+      <c r="AE203">
+        <v>-2</v>
+      </c>
+      <c r="AF203">
+        <v>-2</v>
+      </c>
+      <c r="AG203">
+        <v>2</v>
+      </c>
+      <c r="AH203">
+        <v>-1</v>
+      </c>
+      <c r="AI203">
+        <v>-7</v>
+      </c>
+      <c r="AJ203">
+        <v>-15</v>
+      </c>
+      <c r="AK203">
+        <v>-1</v>
+      </c>
+      <c r="AL203">
+        <v>6</v>
+      </c>
+      <c r="AM203">
+        <v>9</v>
+      </c>
+      <c r="AP203">
+        <v>9</v>
+      </c>
+      <c r="AW203">
+        <v>5</v>
+      </c>
+      <c r="AX203">
+        <v>2</v>
+      </c>
+      <c r="AY203">
+        <v>3</v>
+      </c>
+      <c r="BC203">
+        <v>10</v>
+      </c>
+      <c r="BD203">
+        <v>-11</v>
+      </c>
+      <c r="BE203">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="204" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="D204">
+        <v>3</v>
+      </c>
+      <c r="E204">
+        <v>1</v>
+      </c>
+      <c r="N204">
+        <v>1</v>
+      </c>
+      <c r="O204">
+        <v>1</v>
+      </c>
+      <c r="P204">
+        <v>1</v>
+      </c>
+      <c r="Q204">
+        <v>1</v>
+      </c>
+      <c r="R204">
+        <v>4</v>
+      </c>
+      <c r="S204">
+        <v>2</v>
+      </c>
+      <c r="T204">
+        <v>1</v>
+      </c>
+      <c r="X204">
+        <v>3</v>
+      </c>
+      <c r="Y204">
+        <v>1</v>
+      </c>
+      <c r="Z204">
+        <v>1</v>
+      </c>
+      <c r="AA204">
+        <v>1</v>
+      </c>
+      <c r="AB204">
+        <v>3</v>
+      </c>
+      <c r="AE204">
+        <v>1</v>
+      </c>
+      <c r="AF204">
+        <v>2</v>
+      </c>
+      <c r="AG204">
+        <v>2</v>
+      </c>
+      <c r="AH204">
+        <v>1</v>
+      </c>
+      <c r="AI204">
+        <v>3</v>
+      </c>
+      <c r="AJ204">
+        <v>5</v>
+      </c>
+      <c r="AK204">
+        <v>3</v>
+      </c>
+      <c r="AL204">
+        <v>1</v>
+      </c>
+      <c r="AM204">
+        <v>1</v>
+      </c>
+      <c r="AP204">
+        <v>1</v>
+      </c>
+      <c r="AW204">
+        <v>1</v>
+      </c>
+      <c r="AX204">
+        <v>1</v>
+      </c>
+      <c r="AY204">
+        <v>1</v>
+      </c>
+      <c r="BC204">
+        <v>1</v>
+      </c>
+      <c r="BD204">
+        <v>3</v>
+      </c>
+      <c r="BE204">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="206" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="B206" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="208" spans="1:57" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A208" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B208" s="1">
+        <v>29</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D208" s="1">
+        <v>14</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F208" s="1">
+        <v>23</v>
+      </c>
+      <c r="G208" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H208" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:57" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="B209">
+        <v>20</v>
+      </c>
+      <c r="D209">
+        <v>14</v>
+      </c>
+      <c r="E209" t="s">
+        <v>109</v>
+      </c>
+      <c r="F209">
+        <v>60</v>
+      </c>
+      <c r="G209" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H209" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="D211">
+        <v>20170807</v>
+      </c>
+      <c r="E211">
+        <v>20170808</v>
+      </c>
+      <c r="F211">
+        <v>20170809</v>
+      </c>
+      <c r="G211">
+        <v>20170810</v>
+      </c>
+      <c r="H211">
+        <v>20170811</v>
+      </c>
+      <c r="I211">
+        <v>20170814</v>
+      </c>
+      <c r="J211">
+        <v>20170815</v>
+      </c>
+      <c r="K211">
+        <v>20170816</v>
+      </c>
+      <c r="L211">
+        <v>20170817</v>
+      </c>
+      <c r="M211">
+        <v>20170818</v>
+      </c>
+      <c r="N211">
+        <v>20170821</v>
+      </c>
+      <c r="O211">
+        <v>20170822</v>
+      </c>
+      <c r="P211">
+        <v>20170823</v>
+      </c>
+      <c r="Q211">
+        <v>20170824</v>
+      </c>
+      <c r="R211">
+        <v>20170825</v>
+      </c>
+      <c r="S211">
+        <v>20170828</v>
+      </c>
+      <c r="T211">
+        <v>20170829</v>
+      </c>
+      <c r="U211">
+        <v>20170830</v>
+      </c>
+      <c r="V211">
+        <v>20170831</v>
+      </c>
+      <c r="W211">
+        <v>20170901</v>
+      </c>
+      <c r="X211">
+        <v>20170904</v>
+      </c>
+      <c r="Y211">
+        <v>20170905</v>
+      </c>
+      <c r="Z211">
+        <v>20170906</v>
+      </c>
+      <c r="AA211">
+        <v>20170907</v>
+      </c>
+      <c r="AB211">
+        <v>20170908</v>
+      </c>
+      <c r="AC211">
+        <v>20170911</v>
+      </c>
+      <c r="AD211">
+        <v>20170912</v>
+      </c>
+      <c r="AE211">
+        <v>20170913</v>
+      </c>
+      <c r="AF211">
+        <v>20170914</v>
+      </c>
+      <c r="AG211">
+        <v>20170915</v>
+      </c>
+      <c r="AH211">
+        <v>20170918</v>
+      </c>
+      <c r="AI211">
+        <v>20170919</v>
+      </c>
+      <c r="AJ211">
+        <v>20170920</v>
+      </c>
+      <c r="AK211">
+        <v>20170921</v>
+      </c>
+      <c r="AL211">
+        <v>20170922</v>
+      </c>
+      <c r="AM211">
+        <v>20170925</v>
+      </c>
+      <c r="AN211">
+        <v>20170926</v>
+      </c>
+      <c r="AO211">
+        <v>20170927</v>
+      </c>
+      <c r="AP211">
+        <v>20170928</v>
+      </c>
+      <c r="AQ211">
+        <v>20170929</v>
+      </c>
+      <c r="AR211">
+        <v>20171009</v>
+      </c>
+      <c r="AS211">
+        <v>20171010</v>
+      </c>
+      <c r="AT211">
+        <v>20171011</v>
+      </c>
+      <c r="AU211">
+        <v>20171012</v>
+      </c>
+      <c r="AV211">
+        <v>20171013</v>
+      </c>
+      <c r="AW211">
+        <v>20171016</v>
+      </c>
+      <c r="AX211">
+        <v>20171017</v>
+      </c>
+      <c r="AY211">
+        <v>20171018</v>
+      </c>
+      <c r="AZ211">
+        <v>20171019</v>
+      </c>
+      <c r="BA211">
+        <v>20171020</v>
+      </c>
+      <c r="BB211">
+        <v>20171023</v>
+      </c>
+      <c r="BC211">
+        <v>20171024</v>
+      </c>
+      <c r="BD211">
+        <v>20171025</v>
+      </c>
+      <c r="BE211">
+        <v>20171026</v>
+      </c>
+    </row>
+    <row r="212" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="A212" t="s">
+        <v>119</v>
+      </c>
+      <c r="D212">
+        <v>-12</v>
+      </c>
+      <c r="L212">
+        <v>-20</v>
+      </c>
+      <c r="M212">
+        <v>-4</v>
+      </c>
+      <c r="N212">
+        <v>-1</v>
+      </c>
+      <c r="O212">
+        <v>-19</v>
+      </c>
+      <c r="P212">
+        <v>-1</v>
+      </c>
+      <c r="Q212">
+        <v>-11</v>
+      </c>
+      <c r="R212">
+        <v>-9</v>
+      </c>
+      <c r="T212">
+        <v>22</v>
+      </c>
+      <c r="U212">
+        <v>22</v>
+      </c>
+      <c r="AB212">
+        <v>6</v>
+      </c>
+      <c r="AE212">
+        <v>-8</v>
+      </c>
+      <c r="AF212">
+        <v>8</v>
+      </c>
+      <c r="AG212">
+        <v>3</v>
+      </c>
+      <c r="AI212">
+        <v>-2</v>
+      </c>
+      <c r="AJ212">
+        <v>-6</v>
+      </c>
+      <c r="AK212">
+        <v>24</v>
+      </c>
+      <c r="AL212">
+        <v>5</v>
+      </c>
+      <c r="AM212">
+        <v>6</v>
+      </c>
+      <c r="AO212">
+        <v>18</v>
+      </c>
+      <c r="AP212">
+        <v>-7</v>
+      </c>
+      <c r="AQ212">
+        <v>-4</v>
+      </c>
+      <c r="AR212">
+        <v>9</v>
+      </c>
+      <c r="AT212">
+        <v>-2</v>
+      </c>
+      <c r="AU212">
+        <v>22</v>
+      </c>
+      <c r="AV212">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="213" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="D213">
+        <v>2</v>
+      </c>
+      <c r="L213">
+        <v>4</v>
+      </c>
+      <c r="M213">
+        <v>2</v>
+      </c>
+      <c r="N213">
+        <v>4</v>
+      </c>
+      <c r="O213">
+        <v>4</v>
+      </c>
+      <c r="P213">
+        <v>1</v>
+      </c>
+      <c r="Q213">
+        <v>4</v>
+      </c>
+      <c r="R213">
+        <v>3</v>
+      </c>
+      <c r="T213">
+        <v>1</v>
+      </c>
+      <c r="U213">
+        <v>1</v>
+      </c>
+      <c r="AB213">
+        <v>1</v>
+      </c>
+      <c r="AE213">
+        <v>3</v>
+      </c>
+      <c r="AF213">
+        <v>1</v>
+      </c>
+      <c r="AG213">
+        <v>2</v>
+      </c>
+      <c r="AI213">
+        <v>3</v>
+      </c>
+      <c r="AJ213">
+        <v>1</v>
+      </c>
+      <c r="AK213">
+        <v>1</v>
+      </c>
+      <c r="AL213">
+        <v>3</v>
+      </c>
+      <c r="AM213">
+        <v>1</v>
+      </c>
+      <c r="AO213">
+        <v>1</v>
+      </c>
+      <c r="AP213">
+        <v>3</v>
+      </c>
+      <c r="AQ213">
+        <v>3</v>
+      </c>
+      <c r="AR213">
+        <v>2</v>
+      </c>
+      <c r="AT213">
+        <v>1</v>
+      </c>
+      <c r="AU213">
+        <v>3</v>
+      </c>
+      <c r="AV213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:57" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="D214" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L214" s="1">
+        <v>-22</v>
+      </c>
+      <c r="M214" s="1">
+        <v>0</v>
+      </c>
+      <c r="N214" s="1">
+        <v>1</v>
+      </c>
+      <c r="O214" s="1">
+        <v>-22</v>
+      </c>
+      <c r="Q214" s="1">
+        <v>-10</v>
+      </c>
+      <c r="R214" s="1">
+        <v>-11</v>
+      </c>
+      <c r="S214" s="1">
+        <v>12</v>
+      </c>
+      <c r="T214" s="1">
+        <v>21</v>
+      </c>
+      <c r="U214" s="1">
+        <v>21</v>
+      </c>
+      <c r="V214" s="1">
+        <v>25</v>
+      </c>
+      <c r="Z214" s="1">
+        <v>22</v>
+      </c>
+      <c r="AB214" s="1">
+        <v>-2</v>
+      </c>
+      <c r="AE214" s="1">
+        <v>-12</v>
+      </c>
+      <c r="AF214" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG214" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH214" s="1">
+        <v>-18</v>
+      </c>
+      <c r="AI214" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="B215" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D215">
+        <v>58</v>
+      </c>
+      <c r="H215">
+        <v>9</v>
+      </c>
+      <c r="L215">
+        <v>4</v>
+      </c>
+      <c r="M215">
+        <v>2</v>
+      </c>
+      <c r="N215">
+        <v>3</v>
+      </c>
+      <c r="O215">
+        <v>4</v>
+      </c>
+      <c r="Q215">
+        <v>4</v>
+      </c>
+      <c r="R215">
+        <v>3</v>
+      </c>
+      <c r="S215">
+        <v>1</v>
+      </c>
+      <c r="T215">
+        <v>2</v>
+      </c>
+      <c r="U215">
+        <v>1</v>
+      </c>
+      <c r="V215">
+        <v>1</v>
+      </c>
+      <c r="Z215">
+        <v>2</v>
+      </c>
+      <c r="AB215">
+        <v>2</v>
+      </c>
+      <c r="AE215">
+        <v>2</v>
+      </c>
+      <c r="AF215">
+        <v>2</v>
+      </c>
+      <c r="AG215">
+        <v>2</v>
+      </c>
+      <c r="AH215">
+        <v>5</v>
+      </c>
+      <c r="AI215">
+        <v>2</v>
+      </c>
+      <c r="AO215">
+        <v>13</v>
+      </c>
+      <c r="AP215">
+        <v>-9</v>
+      </c>
+      <c r="AQ215">
+        <v>-6</v>
+      </c>
+      <c r="AR215">
+        <v>6</v>
+      </c>
+      <c r="AS215">
+        <v>35</v>
+      </c>
+      <c r="AT215">
+        <v>-4</v>
+      </c>
+      <c r="AU215">
+        <v>20</v>
+      </c>
+      <c r="AV215">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="216" spans="1:57" x14ac:dyDescent="0.15">
+      <c r="D216">
+        <v>1</v>
+      </c>
+      <c r="H216">
+        <v>1</v>
+      </c>
+      <c r="AO216">
+        <v>1</v>
+      </c>
+      <c r="AP216">
+        <v>3</v>
+      </c>
+      <c r="AQ216">
+        <v>3</v>
+      </c>
+      <c r="AR216">
+        <v>2</v>
+      </c>
+      <c r="AS216">
+        <v>1</v>
+      </c>
+      <c r="AT216">
+        <v>1</v>
+      </c>
+      <c r="AU216">
+        <v>3</v>
+      </c>
+      <c r="AV216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="219" spans="1:57" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A219" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B219" s="1">
+        <v>26</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D219" s="1">
+        <v>14</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F219" s="1">
+        <v>51</v>
+      </c>
+      <c r="G219" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H219" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add the win 10
</commit_message>
<xml_diff>
--- a/python/two_band/回测.xlsx
+++ b/python/two_band/回测.xlsx
@@ -867,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="AJ88" workbookViewId="0">
+      <selection activeCell="BE109" sqref="BE109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>